<commit_message>
revised part numbers in BOM
</commit_message>
<xml_diff>
--- a/hdw/Power_Board/LTC7851_Demo/LTC7851_Demo_bom_.xlsx
+++ b/hdw/Power_Board/LTC7851_Demo/LTC7851_Demo_bom_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Demo Boards\LTC7851_Demo\hdw\LTC7851_Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic_Display\hdw\Power_Board\LTC7851_Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F803F93F-8722-4B94-8CAC-6803440A70A2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A7087A-B876-41D1-AE95-F2947F016697}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC7851_Demo_bom_" sheetId="1" r:id="rId1"/>
@@ -304,9 +304,6 @@
     <t>IPC100N04S51R7ATMA1</t>
   </si>
   <si>
-    <t>BSC123N10LSGATMA1CT-ND</t>
-  </si>
-  <si>
     <t>R301</t>
   </si>
   <si>
@@ -554,12 +551,15 @@
   </si>
   <si>
     <t>SIC779CD-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t>IPC100N04S51R7ATMA1CT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
@@ -1403,11 +1403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1981,13 +1981,13 @@
         <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="2">
         <v>0</v>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="3">
         <v>603</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="2">
         <v>0</v>
@@ -2013,7 +2013,7 @@
         <v>10</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E39" s="3">
         <v>402</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C40" s="2">
         <v>4</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E40" s="3">
         <v>402</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="41" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="2">
         <v>10</v>
@@ -2047,7 +2047,7 @@
         <v>9</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" s="3">
         <v>603</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="42" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42" s="2">
         <v>10</v>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" s="3">
         <v>402</v>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="E43" s="3">
         <v>603</v>
@@ -2089,16 +2089,16 @@
     </row>
     <row r="44" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E44" s="3">
         <v>402</v>
@@ -2106,16 +2106,16 @@
     </row>
     <row r="45" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C45" s="2">
         <v>11</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="3">
         <v>603</v>
@@ -2123,16 +2123,16 @@
     </row>
     <row r="46" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="E46" s="3">
         <v>402</v>
@@ -2140,16 +2140,16 @@
     </row>
     <row r="47" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="E47" s="3">
         <v>402</v>
@@ -2157,16 +2157,16 @@
     </row>
     <row r="48" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C48" s="2">
         <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E48" s="3">
         <v>603</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B49" s="2">
         <v>2</v>
@@ -2183,7 +2183,7 @@
         <v>9</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E49" s="3">
         <v>603</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B50" s="2">
         <v>200</v>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E50" s="3">
         <v>603</v>
@@ -2208,16 +2208,16 @@
     </row>
     <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E51" s="3">
         <v>603</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B52" s="2">
         <v>324</v>
@@ -2234,7 +2234,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E52" s="3">
         <v>402</v>
@@ -2242,16 +2242,16 @@
     </row>
     <row r="53" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C53" s="2">
-        <v>1</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E53" s="3">
         <v>603</v>
@@ -2259,16 +2259,16 @@
     </row>
     <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="E54" s="3">
         <v>603</v>
@@ -2276,16 +2276,16 @@
     </row>
     <row r="55" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C55" s="2">
         <v>6</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E55" s="3">
         <v>2512</v>
@@ -2293,16 +2293,16 @@
     </row>
     <row r="56" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C56" s="2">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="E56" s="3">
         <v>603</v>
@@ -2310,16 +2310,16 @@
     </row>
     <row r="57" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C57" s="2">
-        <v>1</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="E57" s="3">
         <v>402</v>
@@ -2327,16 +2327,16 @@
     </row>
     <row r="58" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2">
+        <v>1</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="E58" s="3">
         <v>402</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="2">
         <v>680</v>
@@ -2353,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E59" s="3">
         <v>603</v>
@@ -2361,16 +2361,16 @@
     </row>
     <row r="60" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C60" s="2">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E60" s="3">
         <v>603</v>
@@ -2378,121 +2378,121 @@
     </row>
     <row r="61" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C61" s="2">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="E61" s="3"/>
     </row>
     <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="C62" s="2">
         <v>3</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E62" s="3"/>
     </row>
     <row r="63" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C63" s="2">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C64" s="2">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C68" s="2">
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E68" s="3"/>
     </row>

</xml_diff>